<commit_message>
Added some description of charts
</commit_message>
<xml_diff>
--- a/Interactive_dashboard/other_findings.xlsx
+++ b/Interactive_dashboard/other_findings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\NISR\Hackathon2023\Interactive_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1E3FC2-4BDF-4AE4-9398-79196BE11DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03327ABA-2E90-4BCD-B114-0CD5DE1CDB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{010EB460-5497-4C99-B6F1-80D82973F95F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="7" xr2:uid="{010EB460-5497-4C99-B6F1-80D82973F95F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF492EB-0C50-4FB9-8A39-6AFFBA543650}">
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3155,8 +3155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F338FB6-06CE-4089-84AB-BEF49E834DD9}">
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3231,7 +3231,7 @@
       <c r="T1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="14" t="s">
         <v>61</v>
       </c>
       <c r="V1" s="8" t="s">

</xml_diff>